<commit_message>
data: update of data for only BA orientation
</commit_message>
<xml_diff>
--- a/data/Timetable_Master_Management.xlsx
+++ b/data/Timetable_Master_Management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteogross/Desktop/Master/BA 3/Programming Tools/GitHub/project--G2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteogross/Desktop/Master/BA 3/Programming Tools/GitHub/project--G2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5354595D-5E82-D043-AABB-874CA6A6E4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1707DE-E77D-4844-B934-E85907030B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14160" xr2:uid="{7D46FA66-D2EE-D643-A8C9-830764CAC309}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="182">
   <si>
     <t xml:space="preserve">Start </t>
   </si>
@@ -132,18 +132,6 @@
     <t>R. Oeuvray</t>
   </si>
   <si>
-    <t>Mandatory SOL</t>
-  </si>
-  <si>
-    <t>Mandatory BEE</t>
-  </si>
-  <si>
-    <t>Because they have to choose either Comp Strat or OTDM (see study plan 2021-2022 for BEE)</t>
-  </si>
-  <si>
-    <t>Mandatory MRKT</t>
-  </si>
-  <si>
     <t>Competitive Advantage &amp; Strategic Interactions</t>
   </si>
   <si>
@@ -303,9 +291,6 @@
     <t>I. Sanders</t>
   </si>
   <si>
-    <t>Aperiodic / Wed and Mon</t>
-  </si>
-  <si>
     <t>Spatial Modelling of Species &amp; Biodiversity</t>
   </si>
   <si>
@@ -570,18 +555,6 @@
     <t>Advanced Programming</t>
   </si>
   <si>
-    <t>BA only</t>
-  </si>
-  <si>
-    <t>SOL only</t>
-  </si>
-  <si>
-    <t>BEE only</t>
-  </si>
-  <si>
-    <t>MRKT only</t>
-  </si>
-  <si>
     <t>BA orientation</t>
   </si>
   <si>
@@ -606,7 +579,7 @@
     <t>Because they have to choose either Evolution of Cooperation or Human Behavior and Evolutionary Interference(see study plan 2021-2022 for BEE)</t>
   </si>
   <si>
-    <t>Class that is assigned to no specific orientation</t>
+    <t>No orientation</t>
   </si>
 </sst>
 </file>
@@ -632,7 +605,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -648,12 +621,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,12 +676,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -723,8 +689,6 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,12 +1003,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEBCED3-0F7A-9D40-B959-B2A6745D0A8C}">
-  <dimension ref="A1:Y99"/>
+  <dimension ref="A1:S99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="X16" sqref="X16"/>
+      <selection pane="bottomLeft" activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1062,15 +1026,13 @@
     <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="12.33203125" customWidth="1"/>
-    <col min="24" max="24" width="78.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="242.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" customWidth="1"/>
+    <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="125.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="242.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1099,49 +1061,31 @@
         <v>1</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1191,31 +1135,10 @@
         <v>0</v>
       </c>
       <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="4">
-        <v>1</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1231,10 +1154,10 @@
       <c r="E3" s="2">
         <v>6</v>
       </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
         <v>0</v>
       </c>
       <c r="H3" s="3">
@@ -1249,44 +1172,26 @@
       <c r="K3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="5">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>1</v>
-      </c>
-      <c r="N3" s="5">
-        <v>1</v>
-      </c>
-      <c r="O3" s="5">
-        <v>1</v>
-      </c>
-      <c r="P3" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>1</v>
-      </c>
-      <c r="R3" s="5">
-        <v>1</v>
-      </c>
-      <c r="S3" s="5">
-        <v>1</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
-        <v>0</v>
-      </c>
-      <c r="W3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1302,10 +1207,10 @@
       <c r="E4" s="2">
         <v>6</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
         <v>0</v>
       </c>
       <c r="H4" s="3">
@@ -1320,44 +1225,26 @@
       <c r="K4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="5">
-        <v>1</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1</v>
-      </c>
-      <c r="P4" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1</v>
-      </c>
-      <c r="R4" s="5">
-        <v>1</v>
-      </c>
-      <c r="S4" s="5">
-        <v>1</v>
-      </c>
-      <c r="T4" s="2">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2">
-        <v>0</v>
-      </c>
-      <c r="V4" s="2">
-        <v>0</v>
-      </c>
-      <c r="W4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1409,26 +1296,8 @@
       <c r="Q5" s="2">
         <v>0</v>
       </c>
-      <c r="R5" s="2">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
-        <v>1</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1475,31 +1344,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1549,31 +1400,10 @@
         <v>0</v>
       </c>
       <c r="Q7" s="2">
-        <v>1</v>
-      </c>
-      <c r="R7" s="4">
-        <v>1</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2">
-        <v>0</v>
-      </c>
-      <c r="V7" s="2">
-        <v>0</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1625,26 +1455,8 @@
       <c r="Q8" s="2">
         <v>0</v>
       </c>
-      <c r="R8" s="2">
-        <v>0</v>
-      </c>
-      <c r="S8" s="2">
-        <v>1</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0</v>
-      </c>
-      <c r="U8" s="2">
-        <v>0</v>
-      </c>
-      <c r="V8" s="2">
-        <v>0</v>
-      </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1696,26 +1508,8 @@
       <c r="Q9" s="2">
         <v>0</v>
       </c>
-      <c r="R9" s="2">
-        <v>1</v>
-      </c>
-      <c r="S9" s="2">
-        <v>0</v>
-      </c>
-      <c r="T9" s="2">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2">
-        <v>0</v>
-      </c>
-      <c r="V9" s="2">
-        <v>0</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>1</v>
       </c>
@@ -1765,31 +1559,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="2">
-        <v>1</v>
-      </c>
-      <c r="R10" s="4">
-        <v>1</v>
-      </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2">
-        <v>0</v>
-      </c>
-      <c r="V10" s="2">
-        <v>0</v>
-      </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-      <c r="X10" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1841,26 +1614,8 @@
       <c r="Q11" s="2">
         <v>0</v>
       </c>
-      <c r="R11" s="2">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2">
-        <v>1</v>
-      </c>
-      <c r="T11" s="2">
-        <v>0</v>
-      </c>
-      <c r="U11" s="2">
-        <v>0</v>
-      </c>
-      <c r="V11" s="2">
-        <v>0</v>
-      </c>
-      <c r="W11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -1912,26 +1667,8 @@
       <c r="Q12" s="2">
         <v>0</v>
       </c>
-      <c r="R12" s="2">
-        <v>1</v>
-      </c>
-      <c r="S12" s="2">
-        <v>0</v>
-      </c>
-      <c r="T12" s="2">
-        <v>0</v>
-      </c>
-      <c r="U12" s="2">
-        <v>0</v>
-      </c>
-      <c r="V12" s="2">
-        <v>0</v>
-      </c>
-      <c r="W12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>1</v>
       </c>
@@ -1978,31 +1715,13 @@
         <v>0</v>
       </c>
       <c r="P13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="2">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2">
-        <v>0</v>
-      </c>
-      <c r="T13" s="2">
-        <v>0</v>
-      </c>
-      <c r="U13" s="2">
-        <v>0</v>
-      </c>
-      <c r="V13" s="2">
-        <v>0</v>
-      </c>
-      <c r="W13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2</v>
       </c>
@@ -2010,10 +1729,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2">
         <v>6</v>
@@ -2054,26 +1773,8 @@
       <c r="Q14" s="2">
         <v>0</v>
       </c>
-      <c r="R14" s="2">
-        <v>0</v>
-      </c>
-      <c r="S14" s="2">
-        <v>0</v>
-      </c>
-      <c r="T14" s="2">
-        <v>0</v>
-      </c>
-      <c r="U14" s="2">
-        <v>0</v>
-      </c>
-      <c r="V14" s="2">
-        <v>0</v>
-      </c>
-      <c r="W14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2</v>
       </c>
@@ -2081,10 +1782,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E15" s="2">
         <v>6</v>
@@ -2125,26 +1826,8 @@
       <c r="Q15" s="2">
         <v>0</v>
       </c>
-      <c r="R15" s="2">
-        <v>0</v>
-      </c>
-      <c r="S15" s="2">
-        <v>0</v>
-      </c>
-      <c r="T15" s="2">
-        <v>0</v>
-      </c>
-      <c r="U15" s="2">
-        <v>0</v>
-      </c>
-      <c r="V15" s="2">
-        <v>0</v>
-      </c>
-      <c r="W15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2</v>
       </c>
@@ -2152,10 +1835,10 @@
         <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2">
         <v>6</v>
@@ -2196,39 +1879,21 @@
       <c r="Q16" s="2">
         <v>0</v>
       </c>
-      <c r="R16" s="2">
-        <v>0</v>
-      </c>
-      <c r="S16" s="2">
-        <v>0</v>
-      </c>
-      <c r="T16" s="2">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2">
-        <v>0</v>
-      </c>
-      <c r="W16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="8">
         <v>1.5</v>
       </c>
       <c r="F17" s="2">
@@ -2237,10 +1902,10 @@
       <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>0.5</v>
       </c>
       <c r="J17" s="2">
@@ -2267,26 +1932,8 @@
       <c r="Q17" s="2">
         <v>0</v>
       </c>
-      <c r="R17" s="2">
-        <v>0</v>
-      </c>
-      <c r="S17" s="2">
-        <v>0</v>
-      </c>
-      <c r="T17" s="2">
-        <v>0</v>
-      </c>
-      <c r="U17" s="2">
-        <v>0</v>
-      </c>
-      <c r="V17" s="2">
-        <v>0</v>
-      </c>
-      <c r="W17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -2294,10 +1941,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E18" s="2">
         <v>6</v>
@@ -2338,26 +1985,8 @@
       <c r="Q18" s="2">
         <v>0</v>
       </c>
-      <c r="R18" s="2">
-        <v>0</v>
-      </c>
-      <c r="S18" s="2">
-        <v>0</v>
-      </c>
-      <c r="T18" s="2">
-        <v>0</v>
-      </c>
-      <c r="U18" s="2">
-        <v>0</v>
-      </c>
-      <c r="V18" s="2">
-        <v>0</v>
-      </c>
-      <c r="W18" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2</v>
       </c>
@@ -2365,10 +1994,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E19" s="2">
         <v>6</v>
@@ -2409,26 +2038,8 @@
       <c r="Q19" s="2">
         <v>0</v>
       </c>
-      <c r="R19" s="2">
-        <v>0</v>
-      </c>
-      <c r="S19" s="2">
-        <v>0</v>
-      </c>
-      <c r="T19" s="2">
-        <v>0</v>
-      </c>
-      <c r="U19" s="2">
-        <v>0</v>
-      </c>
-      <c r="V19" s="2">
-        <v>0</v>
-      </c>
-      <c r="W19" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2</v>
       </c>
@@ -2436,7 +2047,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>16</v>
@@ -2480,26 +2091,8 @@
       <c r="Q20" s="2">
         <v>0</v>
       </c>
-      <c r="R20" s="2">
-        <v>0</v>
-      </c>
-      <c r="S20" s="2">
-        <v>0</v>
-      </c>
-      <c r="T20" s="2">
-        <v>0</v>
-      </c>
-      <c r="U20" s="2">
-        <v>0</v>
-      </c>
-      <c r="V20" s="2">
-        <v>0</v>
-      </c>
-      <c r="W20" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2</v>
       </c>
@@ -2507,10 +2100,10 @@
         <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E21" s="2">
         <v>6</v>
@@ -2551,26 +2144,8 @@
       <c r="Q21" s="2">
         <v>0</v>
       </c>
-      <c r="R21" s="2">
-        <v>0</v>
-      </c>
-      <c r="S21" s="2">
-        <v>0</v>
-      </c>
-      <c r="T21" s="2">
-        <v>0</v>
-      </c>
-      <c r="U21" s="2">
-        <v>0</v>
-      </c>
-      <c r="V21" s="2">
-        <v>0</v>
-      </c>
-      <c r="W21" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2</v>
       </c>
@@ -2578,10 +2153,10 @@
         <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E22" s="2">
         <v>6</v>
@@ -2622,26 +2197,8 @@
       <c r="Q22" s="2">
         <v>0</v>
       </c>
-      <c r="R22" s="2">
-        <v>0</v>
-      </c>
-      <c r="S22" s="2">
-        <v>0</v>
-      </c>
-      <c r="T22" s="2">
-        <v>0</v>
-      </c>
-      <c r="U22" s="2">
-        <v>1</v>
-      </c>
-      <c r="V22" s="2">
-        <v>0</v>
-      </c>
-      <c r="W22" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2</v>
       </c>
@@ -2649,10 +2206,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E23" s="2">
         <v>6</v>
@@ -2693,26 +2250,8 @@
       <c r="Q23" s="2">
         <v>0</v>
       </c>
-      <c r="R23" s="2">
-        <v>0</v>
-      </c>
-      <c r="S23" s="2">
-        <v>1</v>
-      </c>
-      <c r="T23" s="2">
-        <v>0</v>
-      </c>
-      <c r="U23" s="2">
-        <v>0</v>
-      </c>
-      <c r="V23" s="2">
-        <v>0</v>
-      </c>
-      <c r="W23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2</v>
       </c>
@@ -2720,10 +2259,10 @@
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2">
         <v>6</v>
@@ -2764,26 +2303,8 @@
       <c r="Q24" s="2">
         <v>0</v>
       </c>
-      <c r="R24" s="2">
-        <v>0</v>
-      </c>
-      <c r="S24" s="2">
-        <v>0</v>
-      </c>
-      <c r="T24" s="2">
-        <v>0</v>
-      </c>
-      <c r="U24" s="2">
-        <v>0</v>
-      </c>
-      <c r="V24" s="2">
-        <v>0</v>
-      </c>
-      <c r="W24" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2</v>
       </c>
@@ -2791,10 +2312,10 @@
         <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E25" s="2">
         <v>6</v>
@@ -2835,39 +2356,21 @@
       <c r="Q25" s="2">
         <v>0</v>
       </c>
-      <c r="R25" s="2">
-        <v>0</v>
-      </c>
-      <c r="S25" s="2">
-        <v>0</v>
-      </c>
-      <c r="T25" s="2">
-        <v>0</v>
-      </c>
-      <c r="U25" s="2">
-        <v>0</v>
-      </c>
-      <c r="V25" s="2">
-        <v>0</v>
-      </c>
-      <c r="W25" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="9">
+      <c r="C26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="8">
         <v>1.5</v>
       </c>
       <c r="F26" s="2">
@@ -2876,10 +2379,10 @@
       <c r="G26" s="2">
         <v>0</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="7">
         <v>0.5</v>
       </c>
       <c r="J26" s="2">
@@ -2906,26 +2409,8 @@
       <c r="Q26" s="2">
         <v>0</v>
       </c>
-      <c r="R26" s="2">
-        <v>0</v>
-      </c>
-      <c r="S26" s="2">
-        <v>0</v>
-      </c>
-      <c r="T26" s="2">
-        <v>0</v>
-      </c>
-      <c r="U26" s="2">
-        <v>0</v>
-      </c>
-      <c r="V26" s="2">
-        <v>0</v>
-      </c>
-      <c r="W26" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>2</v>
       </c>
@@ -2933,10 +2418,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E27" s="2">
         <v>6</v>
@@ -2959,7 +2444,7 @@
       <c r="K27" s="2">
         <v>0</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L27" s="6">
         <v>0</v>
       </c>
       <c r="M27" s="2">
@@ -2977,26 +2462,8 @@
       <c r="Q27" s="2">
         <v>0</v>
       </c>
-      <c r="R27" s="2">
-        <v>0</v>
-      </c>
-      <c r="S27" s="2">
-        <v>0</v>
-      </c>
-      <c r="T27" s="2">
-        <v>0</v>
-      </c>
-      <c r="U27" s="2">
-        <v>0</v>
-      </c>
-      <c r="V27" s="2">
-        <v>0</v>
-      </c>
-      <c r="W27" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>2</v>
       </c>
@@ -3004,10 +2471,10 @@
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E28" s="2">
         <v>6</v>
@@ -3048,26 +2515,8 @@
       <c r="Q28" s="2">
         <v>0</v>
       </c>
-      <c r="R28" s="2">
-        <v>0</v>
-      </c>
-      <c r="S28" s="2">
-        <v>0</v>
-      </c>
-      <c r="T28" s="2">
-        <v>0</v>
-      </c>
-      <c r="U28" s="2">
-        <v>0</v>
-      </c>
-      <c r="V28" s="2">
-        <v>0</v>
-      </c>
-      <c r="W28" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>2</v>
       </c>
@@ -3075,10 +2524,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E29" s="2">
         <v>3</v>
@@ -3119,26 +2568,8 @@
       <c r="Q29" s="2">
         <v>0</v>
       </c>
-      <c r="R29" s="2">
-        <v>0</v>
-      </c>
-      <c r="S29" s="2">
-        <v>0</v>
-      </c>
-      <c r="T29" s="2">
-        <v>0</v>
-      </c>
-      <c r="U29" s="2">
-        <v>0</v>
-      </c>
-      <c r="V29" s="2">
-        <v>0</v>
-      </c>
-      <c r="W29" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>2</v>
       </c>
@@ -3146,10 +2577,10 @@
         <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
@@ -3190,26 +2621,8 @@
       <c r="Q30" s="2">
         <v>0</v>
       </c>
-      <c r="R30" s="2">
-        <v>0</v>
-      </c>
-      <c r="S30" s="2">
-        <v>0</v>
-      </c>
-      <c r="T30" s="2">
-        <v>0</v>
-      </c>
-      <c r="U30" s="2">
-        <v>1</v>
-      </c>
-      <c r="V30" s="2">
-        <v>0</v>
-      </c>
-      <c r="W30" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>2</v>
       </c>
@@ -3217,10 +2630,10 @@
         <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2">
         <v>6</v>
@@ -3261,37 +2674,19 @@
       <c r="Q31" s="2">
         <v>0</v>
       </c>
-      <c r="R31" s="2">
-        <v>0</v>
-      </c>
-      <c r="S31" s="2">
-        <v>0</v>
-      </c>
-      <c r="T31" s="2">
-        <v>0</v>
-      </c>
-      <c r="U31" s="2">
-        <v>0</v>
-      </c>
-      <c r="V31" s="2">
-        <v>0</v>
-      </c>
-      <c r="W31" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>67</v>
+      <c r="C32" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E32" s="2">
         <v>3</v>
@@ -3332,26 +2727,8 @@
       <c r="Q32" s="2">
         <v>0</v>
       </c>
-      <c r="R32" s="2">
-        <v>0</v>
-      </c>
-      <c r="S32" s="2">
-        <v>0</v>
-      </c>
-      <c r="T32" s="2">
-        <v>0</v>
-      </c>
-      <c r="U32" s="2">
-        <v>0</v>
-      </c>
-      <c r="V32" s="2">
-        <v>0</v>
-      </c>
-      <c r="W32" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>2</v>
       </c>
@@ -3359,10 +2736,10 @@
         <v>9</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E33" s="2">
         <v>6</v>
@@ -3403,26 +2780,8 @@
       <c r="Q33" s="2">
         <v>0</v>
       </c>
-      <c r="R33" s="2">
-        <v>0</v>
-      </c>
-      <c r="S33" s="2">
-        <v>0</v>
-      </c>
-      <c r="T33" s="2">
-        <v>0</v>
-      </c>
-      <c r="U33" s="2">
-        <v>0</v>
-      </c>
-      <c r="V33" s="2">
-        <v>0</v>
-      </c>
-      <c r="W33" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>2</v>
       </c>
@@ -3430,10 +2789,10 @@
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E34" s="2">
         <v>6</v>
@@ -3474,26 +2833,8 @@
       <c r="Q34" s="2">
         <v>0</v>
       </c>
-      <c r="R34" s="2">
-        <v>0</v>
-      </c>
-      <c r="S34" s="2">
-        <v>0</v>
-      </c>
-      <c r="T34" s="2">
-        <v>0</v>
-      </c>
-      <c r="U34" s="2">
-        <v>0</v>
-      </c>
-      <c r="V34" s="2">
-        <v>0</v>
-      </c>
-      <c r="W34" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>2</v>
       </c>
@@ -3501,10 +2842,10 @@
         <v>13</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E35" s="2">
         <v>6</v>
@@ -3545,26 +2886,8 @@
       <c r="Q35" s="2">
         <v>0</v>
       </c>
-      <c r="R35" s="2">
-        <v>0</v>
-      </c>
-      <c r="S35" s="2">
-        <v>0</v>
-      </c>
-      <c r="T35" s="2">
-        <v>0</v>
-      </c>
-      <c r="U35" s="2">
-        <v>0</v>
-      </c>
-      <c r="V35" s="2">
-        <v>0</v>
-      </c>
-      <c r="W35" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>2</v>
       </c>
@@ -3572,10 +2895,10 @@
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E36" s="2">
         <v>6</v>
@@ -3614,26 +2937,8 @@
       <c r="Q36" s="2">
         <v>0</v>
       </c>
-      <c r="R36" s="2">
-        <v>0</v>
-      </c>
-      <c r="S36" s="2">
-        <v>0</v>
-      </c>
-      <c r="T36" s="2">
-        <v>0</v>
-      </c>
-      <c r="U36" s="2">
-        <v>0</v>
-      </c>
-      <c r="V36" s="2">
-        <v>0</v>
-      </c>
-      <c r="W36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -3641,10 +2946,10 @@
         <v>13</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E37" s="2">
         <v>6</v>
@@ -3685,37 +2990,19 @@
       <c r="Q37" s="2">
         <v>0</v>
       </c>
-      <c r="R37" s="2">
-        <v>0</v>
-      </c>
-      <c r="S37" s="2">
-        <v>0</v>
-      </c>
-      <c r="T37" s="2">
-        <v>0</v>
-      </c>
-      <c r="U37" s="2">
-        <v>0</v>
-      </c>
-      <c r="V37" s="2">
-        <v>0</v>
-      </c>
-      <c r="W37" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>74</v>
+      <c r="C38" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E38" s="2">
         <v>3</v>
@@ -3756,37 +3043,19 @@
       <c r="Q38" s="2">
         <v>0</v>
       </c>
-      <c r="R38" s="2">
-        <v>0</v>
-      </c>
-      <c r="S38" s="2">
-        <v>0</v>
-      </c>
-      <c r="T38" s="2">
-        <v>0</v>
-      </c>
-      <c r="U38" s="2">
-        <v>0</v>
-      </c>
-      <c r="V38" s="2">
-        <v>0</v>
-      </c>
-      <c r="W38" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>75</v>
+      <c r="C39" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E39" s="2">
         <v>3</v>
@@ -3827,37 +3096,19 @@
       <c r="Q39" s="2">
         <v>0</v>
       </c>
-      <c r="R39" s="2">
-        <v>0</v>
-      </c>
-      <c r="S39" s="2">
-        <v>0</v>
-      </c>
-      <c r="T39" s="2">
-        <v>0</v>
-      </c>
-      <c r="U39" s="2">
-        <v>0</v>
-      </c>
-      <c r="V39" s="2">
-        <v>0</v>
-      </c>
-      <c r="W39" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="13" t="s">
-        <v>76</v>
+      <c r="C40" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E40" s="2">
         <v>3</v>
@@ -3893,45 +3144,24 @@
         <v>0</v>
       </c>
       <c r="P40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q40" s="2">
         <v>0</v>
       </c>
-      <c r="R40" s="2">
-        <v>0</v>
-      </c>
-      <c r="S40" s="2">
-        <v>0</v>
-      </c>
-      <c r="T40" s="2">
-        <v>0</v>
-      </c>
-      <c r="U40" s="2">
-        <v>0</v>
-      </c>
-      <c r="V40" s="2">
-        <v>0</v>
-      </c>
-      <c r="W40" s="2">
-        <v>0</v>
-      </c>
-      <c r="X40" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>77</v>
+      <c r="C41" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E41" s="2">
         <v>1.5</v>
@@ -3972,37 +3202,19 @@
       <c r="Q41" s="2">
         <v>0</v>
       </c>
-      <c r="R41" s="2">
-        <v>0</v>
-      </c>
-      <c r="S41" s="2">
-        <v>0</v>
-      </c>
-      <c r="T41" s="2">
-        <v>0</v>
-      </c>
-      <c r="U41" s="2">
-        <v>0</v>
-      </c>
-      <c r="V41" s="2">
-        <v>0</v>
-      </c>
-      <c r="W41" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>58</v>
+      <c r="C42" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E42" s="2">
         <v>6</v>
@@ -4043,37 +3255,19 @@
       <c r="Q42" s="2">
         <v>0</v>
       </c>
-      <c r="R42" s="2">
-        <v>0</v>
-      </c>
-      <c r="S42" s="2">
-        <v>0</v>
-      </c>
-      <c r="T42" s="2">
-        <v>0</v>
-      </c>
-      <c r="U42" s="2">
-        <v>0</v>
-      </c>
-      <c r="V42" s="2">
-        <v>0</v>
-      </c>
-      <c r="W42" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>2</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="13" t="s">
-        <v>78</v>
+      <c r="C43" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E43" s="2">
         <v>6</v>
@@ -4109,47 +3303,26 @@
         <v>0</v>
       </c>
       <c r="P43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q43" s="2">
         <v>0</v>
       </c>
-      <c r="R43" s="2">
-        <v>0</v>
-      </c>
-      <c r="S43" s="2">
-        <v>0</v>
-      </c>
-      <c r="T43" s="2">
-        <v>0</v>
-      </c>
-      <c r="U43" s="2">
-        <v>0</v>
-      </c>
-      <c r="V43" s="2">
-        <v>0</v>
-      </c>
-      <c r="W43" s="2">
-        <v>0</v>
-      </c>
-      <c r="X43" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>79</v>
+      <c r="C44" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E44" s="4">
+        <v>84</v>
+      </c>
+      <c r="E44" s="2">
         <v>1.5</v>
       </c>
       <c r="F44" s="2">
@@ -4188,40 +3361,19 @@
       <c r="Q44" s="2">
         <v>0</v>
       </c>
-      <c r="R44" s="2">
-        <v>0</v>
-      </c>
-      <c r="S44" s="2">
-        <v>0</v>
-      </c>
-      <c r="T44" s="2">
-        <v>0</v>
-      </c>
-      <c r="U44" s="2">
-        <v>0</v>
-      </c>
-      <c r="V44" s="2">
-        <v>0</v>
-      </c>
-      <c r="W44" s="2">
-        <v>0</v>
-      </c>
-      <c r="X44" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>90</v>
+      <c r="C45" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E45" s="2">
         <v>3</v>
@@ -4262,37 +3414,19 @@
       <c r="Q45" s="2">
         <v>0</v>
       </c>
-      <c r="R45" s="2">
-        <v>0</v>
-      </c>
-      <c r="S45" s="2">
-        <v>0</v>
-      </c>
-      <c r="T45" s="2">
-        <v>0</v>
-      </c>
-      <c r="U45" s="2">
-        <v>0</v>
-      </c>
-      <c r="V45" s="2">
-        <v>0</v>
-      </c>
-      <c r="W45" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>91</v>
+      <c r="C46" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E46" s="2">
         <v>6</v>
@@ -4333,37 +3467,19 @@
       <c r="Q46" s="2">
         <v>0</v>
       </c>
-      <c r="R46" s="2">
-        <v>0</v>
-      </c>
-      <c r="S46" s="2">
-        <v>0</v>
-      </c>
-      <c r="T46" s="2">
-        <v>0</v>
-      </c>
-      <c r="U46" s="2">
-        <v>0</v>
-      </c>
-      <c r="V46" s="2">
-        <v>0</v>
-      </c>
-      <c r="W46" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>102</v>
+      <c r="C47" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E47" s="2">
         <v>6</v>
@@ -4404,37 +3520,19 @@
       <c r="Q47" s="2">
         <v>0</v>
       </c>
-      <c r="R47" s="2">
-        <v>0</v>
-      </c>
-      <c r="S47" s="2">
-        <v>0</v>
-      </c>
-      <c r="T47" s="2">
-        <v>0</v>
-      </c>
-      <c r="U47" s="2">
-        <v>0</v>
-      </c>
-      <c r="V47" s="2">
-        <v>0</v>
-      </c>
-      <c r="W47" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>2</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>92</v>
+      <c r="C48" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E48" s="2">
         <v>6</v>
@@ -4475,37 +3573,19 @@
       <c r="Q48" s="2">
         <v>0</v>
       </c>
-      <c r="R48" s="2">
-        <v>0</v>
-      </c>
-      <c r="S48" s="2">
-        <v>0</v>
-      </c>
-      <c r="T48" s="2">
-        <v>0</v>
-      </c>
-      <c r="U48" s="2">
-        <v>0</v>
-      </c>
-      <c r="V48" s="2">
-        <v>0</v>
-      </c>
-      <c r="W48" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>93</v>
+      <c r="C49" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -4546,37 +3626,19 @@
       <c r="Q49" s="2">
         <v>0</v>
       </c>
-      <c r="R49" s="2">
-        <v>0</v>
-      </c>
-      <c r="S49" s="2">
-        <v>0</v>
-      </c>
-      <c r="T49" s="2">
-        <v>0</v>
-      </c>
-      <c r="U49" s="2">
-        <v>0</v>
-      </c>
-      <c r="V49" s="2">
-        <v>0</v>
-      </c>
-      <c r="W49" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>94</v>
+      <c r="C50" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E50" s="2">
         <v>3</v>
@@ -4617,37 +3679,19 @@
       <c r="Q50" s="2">
         <v>0</v>
       </c>
-      <c r="R50" s="2">
-        <v>0</v>
-      </c>
-      <c r="S50" s="2">
-        <v>0</v>
-      </c>
-      <c r="T50" s="2">
-        <v>0</v>
-      </c>
-      <c r="U50" s="2">
-        <v>0</v>
-      </c>
-      <c r="V50" s="2">
-        <v>0</v>
-      </c>
-      <c r="W50" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>95</v>
+      <c r="C51" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E51" s="2">
         <v>6</v>
@@ -4683,42 +3727,21 @@
         <v>0</v>
       </c>
       <c r="P51" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q51" s="2">
         <v>0</v>
       </c>
-      <c r="R51" s="2">
-        <v>0</v>
-      </c>
-      <c r="S51" s="2">
-        <v>0</v>
-      </c>
-      <c r="T51" s="2">
-        <v>0</v>
-      </c>
-      <c r="U51" s="2">
-        <v>0</v>
-      </c>
-      <c r="V51" s="2">
-        <v>0</v>
-      </c>
-      <c r="W51" s="2">
-        <v>0</v>
-      </c>
-      <c r="X51" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>96</v>
+      <c r="C52" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>25</v>
@@ -4757,45 +3780,24 @@
         <v>0</v>
       </c>
       <c r="P52" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q52" s="2">
         <v>0</v>
       </c>
-      <c r="R52" s="2">
-        <v>0</v>
-      </c>
-      <c r="S52" s="2">
-        <v>0</v>
-      </c>
-      <c r="T52" s="2">
-        <v>0</v>
-      </c>
-      <c r="U52" s="2">
-        <v>0</v>
-      </c>
-      <c r="V52" s="2">
-        <v>0</v>
-      </c>
-      <c r="W52" s="2">
-        <v>0</v>
-      </c>
-      <c r="X52" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>2</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>103</v>
+      <c r="C53" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E53" s="2">
         <v>6</v>
@@ -4831,42 +3833,24 @@
         <v>0</v>
       </c>
       <c r="P53" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="2">
-        <v>0</v>
-      </c>
-      <c r="R53" s="2">
-        <v>0</v>
-      </c>
-      <c r="S53" s="2">
-        <v>0</v>
-      </c>
-      <c r="T53" s="2">
-        <v>1</v>
-      </c>
-      <c r="U53" s="2">
-        <v>0</v>
-      </c>
-      <c r="V53" s="2">
-        <v>0</v>
-      </c>
-      <c r="W53" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>104</v>
+      <c r="C54" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E54" s="2">
         <v>6</v>
@@ -4902,45 +3886,24 @@
         <v>0</v>
       </c>
       <c r="P54" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q54" s="2">
         <v>0</v>
       </c>
-      <c r="R54" s="2">
-        <v>0</v>
-      </c>
-      <c r="S54" s="2">
-        <v>0</v>
-      </c>
-      <c r="T54" s="2">
-        <v>0</v>
-      </c>
-      <c r="U54" s="2">
-        <v>0</v>
-      </c>
-      <c r="V54" s="2">
-        <v>0</v>
-      </c>
-      <c r="W54" s="2">
-        <v>0</v>
-      </c>
-      <c r="X54" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>105</v>
+      <c r="C55" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E55" s="2">
         <v>3</v>
@@ -4981,37 +3944,19 @@
       <c r="Q55" s="2">
         <v>0</v>
       </c>
-      <c r="R55" s="2">
-        <v>0</v>
-      </c>
-      <c r="S55" s="2">
-        <v>0</v>
-      </c>
-      <c r="T55" s="2">
-        <v>0</v>
-      </c>
-      <c r="U55" s="2">
-        <v>0</v>
-      </c>
-      <c r="V55" s="2">
-        <v>0</v>
-      </c>
-      <c r="W55" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>2</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>106</v>
+      <c r="C56" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E56" s="2">
         <v>3</v>
@@ -5022,10 +3967,10 @@
       <c r="G56" s="2">
         <v>0</v>
       </c>
-      <c r="H56" s="10">
+      <c r="H56" s="9">
         <v>0.52083333333333337</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I56" s="10">
         <v>0.66666666666666663</v>
       </c>
       <c r="J56" s="2">
@@ -5052,34 +3997,16 @@
       <c r="Q56" s="2">
         <v>0</v>
       </c>
-      <c r="R56" s="2">
-        <v>0</v>
-      </c>
-      <c r="S56" s="2">
-        <v>0</v>
-      </c>
-      <c r="T56" s="2">
-        <v>0</v>
-      </c>
-      <c r="U56" s="2">
-        <v>0</v>
-      </c>
-      <c r="V56" s="2">
-        <v>0</v>
-      </c>
-      <c r="W56" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>107</v>
+      <c r="C57" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>25</v>
@@ -5093,10 +4020,10 @@
       <c r="G57" s="2">
         <v>0</v>
       </c>
-      <c r="H57" s="10">
+      <c r="H57" s="9">
         <v>0.52083333333333337</v>
       </c>
-      <c r="I57" s="11">
+      <c r="I57" s="10">
         <v>0.66666666666666663</v>
       </c>
       <c r="J57" s="2">
@@ -5123,43 +4050,25 @@
       <c r="Q57" s="2">
         <v>0</v>
       </c>
-      <c r="R57" s="4">
-        <v>1</v>
-      </c>
-      <c r="S57" s="2">
-        <v>0</v>
-      </c>
-      <c r="T57" s="2">
-        <v>0</v>
-      </c>
-      <c r="U57" s="2">
-        <v>0</v>
-      </c>
-      <c r="V57" s="2">
-        <v>0</v>
-      </c>
-      <c r="W57" s="2">
-        <v>0</v>
-      </c>
-      <c r="X57" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="Y57" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="R57" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="S57" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="E58" s="2">
         <v>3</v>
@@ -5200,37 +4109,19 @@
       <c r="Q58" s="2">
         <v>0</v>
       </c>
-      <c r="R58" s="2">
-        <v>0</v>
-      </c>
-      <c r="S58" s="2">
-        <v>0</v>
-      </c>
-      <c r="T58" s="2">
-        <v>0</v>
-      </c>
-      <c r="U58" s="2">
-        <v>0</v>
-      </c>
-      <c r="V58" s="2">
-        <v>0</v>
-      </c>
-      <c r="W58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>70</v>
+      <c r="C59" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E59" s="2">
         <v>6</v>
@@ -5271,37 +4162,19 @@
       <c r="Q59" s="2">
         <v>0</v>
       </c>
-      <c r="R59" s="2">
-        <v>0</v>
-      </c>
-      <c r="S59" s="2">
-        <v>0</v>
-      </c>
-      <c r="T59" s="2">
-        <v>0</v>
-      </c>
-      <c r="U59" s="2">
-        <v>0</v>
-      </c>
-      <c r="V59" s="2">
-        <v>0</v>
-      </c>
-      <c r="W59" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>109</v>
+      <c r="C60" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E60" s="2">
         <v>6</v>
@@ -5342,37 +4215,19 @@
       <c r="Q60" s="2">
         <v>0</v>
       </c>
-      <c r="R60" s="2">
-        <v>0</v>
-      </c>
-      <c r="S60" s="2">
-        <v>1</v>
-      </c>
-      <c r="T60" s="2">
-        <v>0</v>
-      </c>
-      <c r="U60" s="2">
-        <v>0</v>
-      </c>
-      <c r="V60" s="2">
-        <v>0</v>
-      </c>
-      <c r="W60" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>42</v>
+      <c r="C61" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E61" s="2">
         <v>6</v>
@@ -5413,37 +4268,19 @@
       <c r="Q61" s="2">
         <v>0</v>
       </c>
-      <c r="R61" s="2">
-        <v>0</v>
-      </c>
-      <c r="S61" s="2">
-        <v>0</v>
-      </c>
-      <c r="T61" s="2">
-        <v>0</v>
-      </c>
-      <c r="U61" s="2">
-        <v>0</v>
-      </c>
-      <c r="V61" s="2">
-        <v>0</v>
-      </c>
-      <c r="W61" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>3</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>120</v>
+      <c r="C62" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E62" s="2">
         <v>3</v>
@@ -5479,45 +4316,24 @@
         <v>0</v>
       </c>
       <c r="P62" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q62" s="2">
         <v>0</v>
       </c>
-      <c r="R62" s="2">
-        <v>0</v>
-      </c>
-      <c r="S62" s="2">
-        <v>0</v>
-      </c>
-      <c r="T62" s="2">
-        <v>0</v>
-      </c>
-      <c r="U62" s="2">
-        <v>0</v>
-      </c>
-      <c r="V62" s="2">
-        <v>0</v>
-      </c>
-      <c r="W62" s="2">
-        <v>0</v>
-      </c>
-      <c r="X62" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>3</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>115</v>
+      <c r="C63" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E63" s="2">
         <v>6</v>
@@ -5558,37 +4374,19 @@
       <c r="Q63" s="2">
         <v>0</v>
       </c>
-      <c r="R63" s="2">
-        <v>0</v>
-      </c>
-      <c r="S63" s="2">
-        <v>0</v>
-      </c>
-      <c r="T63" s="2">
-        <v>0</v>
-      </c>
-      <c r="U63" s="2">
-        <v>0</v>
-      </c>
-      <c r="V63" s="2">
-        <v>0</v>
-      </c>
-      <c r="W63" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>3</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>116</v>
+      <c r="C64" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E64" s="2">
         <v>3</v>
@@ -5629,37 +4427,19 @@
       <c r="Q64" s="2">
         <v>0</v>
       </c>
-      <c r="R64" s="2">
-        <v>0</v>
-      </c>
-      <c r="S64" s="2">
-        <v>0</v>
-      </c>
-      <c r="T64" s="2">
-        <v>0</v>
-      </c>
-      <c r="U64" s="2">
-        <v>0</v>
-      </c>
-      <c r="V64" s="2">
-        <v>0</v>
-      </c>
-      <c r="W64" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>3</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>117</v>
+      <c r="C65" s="4" t="s">
+        <v>112</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E65" s="2">
         <v>6</v>
@@ -5700,37 +4480,19 @@
       <c r="Q65" s="2">
         <v>0</v>
       </c>
-      <c r="R65" s="2">
-        <v>0</v>
-      </c>
-      <c r="S65" s="2">
-        <v>0</v>
-      </c>
-      <c r="T65" s="2">
-        <v>0</v>
-      </c>
-      <c r="U65" s="2">
-        <v>0</v>
-      </c>
-      <c r="V65" s="2">
-        <v>0</v>
-      </c>
-      <c r="W65" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>3</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D66" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="E66" s="2">
         <v>3</v>
@@ -5771,26 +4533,8 @@
       <c r="Q66" s="2">
         <v>0</v>
       </c>
-      <c r="R66" s="2">
-        <v>0</v>
-      </c>
-      <c r="S66" s="2">
-        <v>0</v>
-      </c>
-      <c r="T66" s="2">
-        <v>0</v>
-      </c>
-      <c r="U66" s="2">
-        <v>0</v>
-      </c>
-      <c r="V66" s="2">
-        <v>0</v>
-      </c>
-      <c r="W66" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>3</v>
       </c>
@@ -5798,10 +4542,10 @@
         <v>6</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E67" s="2">
         <v>6</v>
@@ -5842,26 +4586,8 @@
       <c r="Q67" s="2">
         <v>0</v>
       </c>
-      <c r="R67" s="2">
-        <v>0</v>
-      </c>
-      <c r="S67" s="2">
-        <v>0</v>
-      </c>
-      <c r="T67" s="2">
-        <v>0</v>
-      </c>
-      <c r="U67" s="2">
-        <v>0</v>
-      </c>
-      <c r="V67" s="2">
-        <v>0</v>
-      </c>
-      <c r="W67" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>3</v>
       </c>
@@ -5869,10 +4595,10 @@
         <v>9</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E68" s="2">
         <v>6</v>
@@ -5913,26 +4639,8 @@
       <c r="Q68" s="2">
         <v>0</v>
       </c>
-      <c r="R68" s="2">
-        <v>0</v>
-      </c>
-      <c r="S68" s="2">
-        <v>0</v>
-      </c>
-      <c r="T68" s="2">
-        <v>0</v>
-      </c>
-      <c r="U68" s="2">
-        <v>0</v>
-      </c>
-      <c r="V68" s="2">
-        <v>0</v>
-      </c>
-      <c r="W68" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>3</v>
       </c>
@@ -5940,10 +4648,10 @@
         <v>9</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E69" s="2">
         <v>6</v>
@@ -5984,26 +4692,8 @@
       <c r="Q69" s="2">
         <v>0</v>
       </c>
-      <c r="R69" s="2">
-        <v>0</v>
-      </c>
-      <c r="S69" s="2">
-        <v>0</v>
-      </c>
-      <c r="T69" s="2">
-        <v>0</v>
-      </c>
-      <c r="U69" s="2">
-        <v>0</v>
-      </c>
-      <c r="V69" s="2">
-        <v>0</v>
-      </c>
-      <c r="W69" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>3</v>
       </c>
@@ -6011,10 +4701,10 @@
         <v>9</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E70" s="2">
         <v>1.5</v>
@@ -6055,37 +4745,19 @@
       <c r="Q70" s="2">
         <v>0</v>
       </c>
-      <c r="R70" s="2">
-        <v>0</v>
-      </c>
-      <c r="S70" s="2">
-        <v>0</v>
-      </c>
-      <c r="T70" s="2">
-        <v>0</v>
-      </c>
-      <c r="U70" s="2">
-        <v>0</v>
-      </c>
-      <c r="V70" s="2">
-        <v>0</v>
-      </c>
-      <c r="W70" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>128</v>
+      <c r="C71" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E71" s="2">
         <v>6</v>
@@ -6126,39 +4798,21 @@
       <c r="Q71" s="2">
         <v>0</v>
       </c>
-      <c r="R71" s="2">
-        <v>0</v>
-      </c>
-      <c r="S71" s="2">
-        <v>0</v>
-      </c>
-      <c r="T71" s="2">
-        <v>0</v>
-      </c>
-      <c r="U71" s="2">
-        <v>0</v>
-      </c>
-      <c r="V71" s="2">
-        <v>0</v>
-      </c>
-      <c r="W71" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>3</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E72" s="12">
+      <c r="C72" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E72" s="11">
         <v>1.5</v>
       </c>
       <c r="F72" s="2">
@@ -6197,37 +4851,19 @@
       <c r="Q72" s="2">
         <v>0</v>
       </c>
-      <c r="R72" s="2">
-        <v>0</v>
-      </c>
-      <c r="S72" s="2">
-        <v>0</v>
-      </c>
-      <c r="T72" s="2">
-        <v>0</v>
-      </c>
-      <c r="U72" s="2">
-        <v>0</v>
-      </c>
-      <c r="V72" s="2">
-        <v>0</v>
-      </c>
-      <c r="W72" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>3</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="13" t="s">
-        <v>130</v>
+      <c r="C73" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E73" s="2">
         <v>3</v>
@@ -6263,45 +4899,24 @@
         <v>0</v>
       </c>
       <c r="P73" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q73" s="2">
         <v>0</v>
       </c>
-      <c r="R73" s="2">
-        <v>0</v>
-      </c>
-      <c r="S73" s="2">
-        <v>0</v>
-      </c>
-      <c r="T73" s="2">
-        <v>0</v>
-      </c>
-      <c r="U73" s="2">
-        <v>0</v>
-      </c>
-      <c r="V73" s="2">
-        <v>0</v>
-      </c>
-      <c r="W73" s="2">
-        <v>0</v>
-      </c>
-      <c r="X73" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>3</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>138</v>
+      <c r="C74" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="E74" s="2">
         <v>3</v>
@@ -6337,42 +4952,24 @@
         <v>0</v>
       </c>
       <c r="P74" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q74" s="2">
-        <v>0</v>
-      </c>
-      <c r="R74" s="2">
-        <v>0</v>
-      </c>
-      <c r="S74" s="2">
-        <v>0</v>
-      </c>
-      <c r="T74" s="2">
-        <v>1</v>
-      </c>
-      <c r="U74" s="2">
-        <v>0</v>
-      </c>
-      <c r="V74" s="2">
-        <v>0</v>
-      </c>
-      <c r="W74" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>3</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>132</v>
+      <c r="C75" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E75" s="2">
         <v>6</v>
@@ -6413,37 +5010,19 @@
       <c r="Q75" s="2">
         <v>0</v>
       </c>
-      <c r="R75" s="2">
-        <v>0</v>
-      </c>
-      <c r="S75" s="2">
-        <v>0</v>
-      </c>
-      <c r="T75" s="2">
-        <v>0</v>
-      </c>
-      <c r="U75" s="2">
-        <v>0</v>
-      </c>
-      <c r="V75" s="2">
-        <v>0</v>
-      </c>
-      <c r="W75" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>3</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>140</v>
+      <c r="C76" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E76" s="2">
         <v>3</v>
@@ -6484,37 +5063,19 @@
       <c r="Q76" s="2">
         <v>0</v>
       </c>
-      <c r="R76" s="2">
-        <v>0</v>
-      </c>
-      <c r="S76" s="2">
-        <v>0</v>
-      </c>
-      <c r="T76" s="2">
-        <v>0</v>
-      </c>
-      <c r="U76" s="2">
-        <v>0</v>
-      </c>
-      <c r="V76" s="2">
-        <v>0</v>
-      </c>
-      <c r="W76" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>3</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>150</v>
+      <c r="C77" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="E77" s="2">
         <v>6</v>
@@ -6555,37 +5116,19 @@
       <c r="Q77" s="2">
         <v>0</v>
       </c>
-      <c r="R77" s="2">
-        <v>0</v>
-      </c>
-      <c r="S77" s="2">
-        <v>0</v>
-      </c>
-      <c r="T77" s="2">
-        <v>0</v>
-      </c>
-      <c r="U77" s="2">
-        <v>0</v>
-      </c>
-      <c r="V77" s="2">
-        <v>0</v>
-      </c>
-      <c r="W77" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>3</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>142</v>
+      <c r="C78" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E78" s="2">
         <v>6</v>
@@ -6626,37 +5169,19 @@
       <c r="Q78" s="2">
         <v>0</v>
       </c>
-      <c r="R78" s="2">
-        <v>0</v>
-      </c>
-      <c r="S78" s="2">
-        <v>0</v>
-      </c>
-      <c r="T78" s="2">
-        <v>0</v>
-      </c>
-      <c r="U78" s="2">
-        <v>0</v>
-      </c>
-      <c r="V78" s="2">
-        <v>0</v>
-      </c>
-      <c r="W78" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>3</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>143</v>
+      <c r="C79" s="4" t="s">
+        <v>138</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E79" s="2">
         <v>3</v>
@@ -6697,37 +5222,19 @@
       <c r="Q79" s="2">
         <v>0</v>
       </c>
-      <c r="R79" s="2">
-        <v>0</v>
-      </c>
-      <c r="S79" s="2">
-        <v>0</v>
-      </c>
-      <c r="T79" s="2">
-        <v>0</v>
-      </c>
-      <c r="U79" s="2">
-        <v>0</v>
-      </c>
-      <c r="V79" s="2">
-        <v>0</v>
-      </c>
-      <c r="W79" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>3</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>144</v>
+      <c r="C80" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E80" s="2">
         <v>3</v>
@@ -6768,37 +5275,19 @@
       <c r="Q80" s="2">
         <v>0</v>
       </c>
-      <c r="R80" s="2">
-        <v>0</v>
-      </c>
-      <c r="S80" s="2">
-        <v>0</v>
-      </c>
-      <c r="T80" s="2">
-        <v>0</v>
-      </c>
-      <c r="U80" s="2">
-        <v>0</v>
-      </c>
-      <c r="V80" s="2">
-        <v>0</v>
-      </c>
-      <c r="W80" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>3</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>152</v>
+      <c r="C81" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="E81" s="2">
         <v>6</v>
@@ -6839,37 +5328,19 @@
       <c r="Q81" s="2">
         <v>0</v>
       </c>
-      <c r="R81" s="2">
-        <v>0</v>
-      </c>
-      <c r="S81" s="2">
-        <v>0</v>
-      </c>
-      <c r="T81" s="2">
-        <v>0</v>
-      </c>
-      <c r="U81" s="2">
-        <v>0</v>
-      </c>
-      <c r="V81" s="2">
-        <v>0</v>
-      </c>
-      <c r="W81" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>146</v>
+      <c r="C82" s="4" t="s">
+        <v>141</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E82" s="2">
         <v>6</v>
@@ -6910,40 +5381,22 @@
       <c r="Q82" s="2">
         <v>0</v>
       </c>
-      <c r="R82" s="4">
-        <v>1</v>
-      </c>
-      <c r="S82" s="2">
-        <v>0</v>
-      </c>
-      <c r="T82" s="2">
-        <v>0</v>
-      </c>
-      <c r="U82" s="2">
-        <v>0</v>
-      </c>
-      <c r="V82" s="2">
-        <v>0</v>
-      </c>
-      <c r="W82" s="2">
-        <v>0</v>
-      </c>
-      <c r="X82" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="R82" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>3</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>153</v>
+      <c r="C83" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="E83" s="2">
         <v>6</v>
@@ -6979,45 +5432,24 @@
         <v>0</v>
       </c>
       <c r="P83" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q83" s="2">
         <v>0</v>
       </c>
-      <c r="R83" s="2">
-        <v>0</v>
-      </c>
-      <c r="S83" s="2">
-        <v>0</v>
-      </c>
-      <c r="T83" s="2">
-        <v>0</v>
-      </c>
-      <c r="U83" s="2">
-        <v>0</v>
-      </c>
-      <c r="V83" s="2">
-        <v>0</v>
-      </c>
-      <c r="W83" s="2">
-        <v>0</v>
-      </c>
-      <c r="X83" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>3</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>148</v>
+      <c r="C84" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E84" s="2">
         <v>6</v>
@@ -7058,37 +5490,19 @@
       <c r="Q84" s="2">
         <v>0</v>
       </c>
-      <c r="R84" s="2">
-        <v>0</v>
-      </c>
-      <c r="S84" s="2">
-        <v>0</v>
-      </c>
-      <c r="T84" s="2">
-        <v>0</v>
-      </c>
-      <c r="U84" s="2">
-        <v>0</v>
-      </c>
-      <c r="V84" s="2">
-        <v>0</v>
-      </c>
-      <c r="W84" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>3</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="13" t="s">
-        <v>149</v>
+      <c r="C85" s="4" t="s">
+        <v>144</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E85" s="2">
         <v>3</v>
@@ -7124,45 +5538,24 @@
         <v>0</v>
       </c>
       <c r="P85" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q85" s="2">
         <v>0</v>
       </c>
-      <c r="R85" s="2">
-        <v>0</v>
-      </c>
-      <c r="S85" s="2">
-        <v>0</v>
-      </c>
-      <c r="T85" s="2">
-        <v>0</v>
-      </c>
-      <c r="U85" s="2">
-        <v>0</v>
-      </c>
-      <c r="V85" s="2">
-        <v>0</v>
-      </c>
-      <c r="W85" s="2">
-        <v>0</v>
-      </c>
-      <c r="X85" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>3</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>156</v>
+      <c r="C86" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E86" s="2">
         <v>6</v>
@@ -7173,10 +5566,10 @@
       <c r="G86" s="2">
         <v>0</v>
       </c>
-      <c r="H86" s="10">
+      <c r="H86" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I86" s="11">
+      <c r="I86" s="10">
         <v>0.5</v>
       </c>
       <c r="J86" s="2">
@@ -7203,37 +5596,19 @@
       <c r="Q86" s="2">
         <v>0</v>
       </c>
-      <c r="R86" s="2">
-        <v>0</v>
-      </c>
-      <c r="S86" s="2">
-        <v>0</v>
-      </c>
-      <c r="T86" s="2">
-        <v>0</v>
-      </c>
-      <c r="U86" s="2">
-        <v>0</v>
-      </c>
-      <c r="V86" s="2">
-        <v>0</v>
-      </c>
-      <c r="W86" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>3</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>157</v>
+      <c r="C87" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E87" s="2">
         <v>6</v>
@@ -7274,37 +5649,19 @@
       <c r="Q87" s="2">
         <v>0</v>
       </c>
-      <c r="R87" s="2">
-        <v>0</v>
-      </c>
-      <c r="S87" s="2">
-        <v>0</v>
-      </c>
-      <c r="T87" s="2">
-        <v>0</v>
-      </c>
-      <c r="U87" s="2">
-        <v>0</v>
-      </c>
-      <c r="V87" s="2">
-        <v>0</v>
-      </c>
-      <c r="W87" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>3</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>158</v>
+      <c r="C88" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E88" s="2">
         <v>6</v>
@@ -7345,37 +5702,19 @@
       <c r="Q88" s="2">
         <v>0</v>
       </c>
-      <c r="R88" s="2">
-        <v>0</v>
-      </c>
-      <c r="S88" s="2">
-        <v>0</v>
-      </c>
-      <c r="T88" s="2">
-        <v>0</v>
-      </c>
-      <c r="U88" s="2">
-        <v>0</v>
-      </c>
-      <c r="V88" s="2">
-        <v>0</v>
-      </c>
-      <c r="W88" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>3</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>159</v>
+      <c r="C89" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E89" s="2">
         <v>3</v>
@@ -7416,37 +5755,19 @@
       <c r="Q89" s="2">
         <v>0</v>
       </c>
-      <c r="R89" s="2">
-        <v>0</v>
-      </c>
-      <c r="S89" s="2">
-        <v>0</v>
-      </c>
-      <c r="T89" s="2">
-        <v>0</v>
-      </c>
-      <c r="U89" s="2">
-        <v>0</v>
-      </c>
-      <c r="V89" s="2">
-        <v>0</v>
-      </c>
-      <c r="W89" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>3</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="13" t="s">
-        <v>160</v>
+      <c r="C90" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E90" s="2">
         <v>3</v>
@@ -7482,45 +5803,24 @@
         <v>0</v>
       </c>
       <c r="P90" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q90" s="2">
         <v>0</v>
       </c>
-      <c r="R90" s="2">
-        <v>0</v>
-      </c>
-      <c r="S90" s="2">
-        <v>0</v>
-      </c>
-      <c r="T90" s="2">
-        <v>0</v>
-      </c>
-      <c r="U90" s="2">
-        <v>0</v>
-      </c>
-      <c r="V90" s="2">
-        <v>0</v>
-      </c>
-      <c r="W90" s="2">
-        <v>0</v>
-      </c>
-      <c r="X90" s="14" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>3</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>161</v>
+      <c r="C91" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E91" s="2">
         <v>6</v>
@@ -7561,37 +5861,19 @@
       <c r="Q91" s="2">
         <v>0</v>
       </c>
-      <c r="R91" s="2">
-        <v>0</v>
-      </c>
-      <c r="S91" s="2">
-        <v>0</v>
-      </c>
-      <c r="T91" s="2">
-        <v>0</v>
-      </c>
-      <c r="U91" s="2">
-        <v>0</v>
-      </c>
-      <c r="V91" s="2">
-        <v>0</v>
-      </c>
-      <c r="W91" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>3</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>162</v>
+      <c r="C92" s="4" t="s">
+        <v>157</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E92" s="2">
         <v>3</v>
@@ -7632,26 +5914,8 @@
       <c r="Q92" s="2">
         <v>0</v>
       </c>
-      <c r="R92" s="2">
-        <v>0</v>
-      </c>
-      <c r="S92" s="2">
-        <v>0</v>
-      </c>
-      <c r="T92" s="2">
-        <v>0</v>
-      </c>
-      <c r="U92" s="2">
-        <v>0</v>
-      </c>
-      <c r="V92" s="2">
-        <v>0</v>
-      </c>
-      <c r="W92" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>3</v>
       </c>
@@ -7659,10 +5923,10 @@
         <v>18</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E93" s="2">
         <v>3</v>
@@ -7703,26 +5967,8 @@
       <c r="Q93" s="2">
         <v>0</v>
       </c>
-      <c r="R93" s="2">
-        <v>0</v>
-      </c>
-      <c r="S93" s="2">
-        <v>0</v>
-      </c>
-      <c r="T93" s="2">
-        <v>0</v>
-      </c>
-      <c r="U93" s="2">
-        <v>0</v>
-      </c>
-      <c r="V93" s="2">
-        <v>0</v>
-      </c>
-      <c r="W93" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>3</v>
       </c>
@@ -7730,10 +5976,10 @@
         <v>26</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E94" s="2">
         <v>6</v>
@@ -7774,26 +6020,8 @@
       <c r="Q94" s="2">
         <v>0</v>
       </c>
-      <c r="R94" s="2">
-        <v>0</v>
-      </c>
-      <c r="S94" s="2">
-        <v>0</v>
-      </c>
-      <c r="T94" s="2">
-        <v>0</v>
-      </c>
-      <c r="U94" s="2">
-        <v>0</v>
-      </c>
-      <c r="V94" s="2">
-        <v>0</v>
-      </c>
-      <c r="W94" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>3</v>
       </c>
@@ -7801,10 +6029,10 @@
         <v>26</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E95" s="2">
         <v>3</v>
@@ -7845,26 +6073,8 @@
       <c r="Q95" s="2">
         <v>0</v>
       </c>
-      <c r="R95" s="2">
-        <v>0</v>
-      </c>
-      <c r="S95" s="2">
-        <v>0</v>
-      </c>
-      <c r="T95" s="2">
-        <v>0</v>
-      </c>
-      <c r="U95" s="2">
-        <v>0</v>
-      </c>
-      <c r="V95" s="2">
-        <v>0</v>
-      </c>
-      <c r="W95" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>3</v>
       </c>
@@ -7872,10 +6082,10 @@
         <v>26</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E96" s="2">
         <v>6</v>
@@ -7916,26 +6126,8 @@
       <c r="Q96" s="2">
         <v>0</v>
       </c>
-      <c r="R96" s="2">
-        <v>0</v>
-      </c>
-      <c r="S96" s="2">
-        <v>0</v>
-      </c>
-      <c r="T96" s="2">
-        <v>0</v>
-      </c>
-      <c r="U96" s="2">
-        <v>0</v>
-      </c>
-      <c r="V96" s="2">
-        <v>0</v>
-      </c>
-      <c r="W96" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>3</v>
       </c>
@@ -7943,10 +6135,10 @@
         <v>26</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E97" s="2">
         <v>3</v>
@@ -7987,26 +6179,8 @@
       <c r="Q97" s="2">
         <v>0</v>
       </c>
-      <c r="R97" s="2">
-        <v>0</v>
-      </c>
-      <c r="S97" s="2">
-        <v>0</v>
-      </c>
-      <c r="T97" s="2">
-        <v>0</v>
-      </c>
-      <c r="U97" s="2">
-        <v>0</v>
-      </c>
-      <c r="V97" s="2">
-        <v>0</v>
-      </c>
-      <c r="W97" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>3</v>
       </c>
@@ -8014,10 +6188,10 @@
         <v>26</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E98" s="2">
         <v>3</v>
@@ -8058,26 +6232,8 @@
       <c r="Q98" s="2">
         <v>0</v>
       </c>
-      <c r="R98" s="2">
-        <v>0</v>
-      </c>
-      <c r="S98" s="2">
-        <v>0</v>
-      </c>
-      <c r="T98" s="2">
-        <v>0</v>
-      </c>
-      <c r="U98" s="2">
-        <v>0</v>
-      </c>
-      <c r="V98" s="2">
-        <v>0</v>
-      </c>
-      <c r="W98" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>3</v>
       </c>
@@ -8085,10 +6241,10 @@
         <v>26</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E99" s="2">
         <v>6</v>
@@ -8127,24 +6283,6 @@
         <v>0</v>
       </c>
       <c r="Q99" s="2">
-        <v>0</v>
-      </c>
-      <c r="R99" s="2">
-        <v>0</v>
-      </c>
-      <c r="S99" s="2">
-        <v>0</v>
-      </c>
-      <c r="T99" s="2">
-        <v>0</v>
-      </c>
-      <c r="U99" s="2">
-        <v>0</v>
-      </c>
-      <c r="V99" s="2">
-        <v>0</v>
-      </c>
-      <c r="W99" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>